<commit_message>
updated planning and relocated UML diagram from P2 document
</commit_message>
<xml_diff>
--- a/Reports/Thesis Planning.xlsx
+++ b/Reports/Thesis Planning.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Plan</t>
   </si>
@@ -349,7 +349,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -396,9 +396,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -6581,8 +6578,8 @@
   </sheetPr>
   <dimension ref="A2:AM34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:AN35"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -6615,16 +6612,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
       <c r="F3" s="4"/>
       <c r="AA3" s="12"/>
       <c r="AD3" s="1"/>
@@ -6635,9 +6632,9 @@
       <c r="AI3" s="6"/>
     </row>
     <row r="4" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
       <c r="H4" s="7"/>
       <c r="I4" s="12" t="s">
         <v>0</v>
@@ -6681,106 +6678,106 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>46</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>47</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>48</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="17">
         <v>49</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="17">
         <v>50</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="17">
         <v>51</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="17">
         <v>52</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>53</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="17">
         <v>1</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="17">
         <v>2</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="17">
         <v>3</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="17">
         <v>4</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="17">
         <v>5</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="17">
         <v>6</v>
       </c>
-      <c r="T8" s="18">
+      <c r="T8" s="17">
         <v>7</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="17">
         <v>8</v>
       </c>
-      <c r="V8" s="18">
+      <c r="V8" s="17">
         <v>9</v>
       </c>
-      <c r="W8" s="18">
+      <c r="W8" s="17">
         <v>10</v>
       </c>
-      <c r="X8" s="18">
+      <c r="X8" s="17">
         <v>11</v>
       </c>
-      <c r="Y8" s="18">
+      <c r="Y8" s="17">
         <v>12</v>
       </c>
-      <c r="Z8" s="18">
+      <c r="Z8" s="17">
         <v>13</v>
       </c>
-      <c r="AA8" s="18">
+      <c r="AA8" s="17">
         <v>14</v>
       </c>
-      <c r="AB8" s="18">
+      <c r="AB8" s="17">
         <v>15</v>
       </c>
-      <c r="AC8" s="18">
+      <c r="AC8" s="17">
         <v>16</v>
       </c>
-      <c r="AD8" s="18">
+      <c r="AD8" s="17">
         <v>17</v>
       </c>
-      <c r="AE8" s="18">
+      <c r="AE8" s="17">
         <v>18</v>
       </c>
-      <c r="AF8" s="18">
+      <c r="AF8" s="17">
         <v>19</v>
       </c>
-      <c r="AG8" s="18">
+      <c r="AG8" s="17">
         <v>20</v>
       </c>
-      <c r="AH8" s="18">
+      <c r="AH8" s="17">
         <v>21</v>
       </c>
-      <c r="AI8" s="18">
+      <c r="AI8" s="17">
         <v>22</v>
       </c>
-      <c r="AJ8" s="18">
+      <c r="AJ8" s="17">
         <v>23</v>
       </c>
-      <c r="AK8" s="18">
+      <c r="AK8" s="17">
         <v>24</v>
       </c>
-      <c r="AL8" s="18">
+      <c r="AL8" s="17">
         <v>25</v>
       </c>
-      <c r="AM8" s="18">
+      <c r="AM8" s="17">
         <v>26</v>
       </c>
     </row>
@@ -6837,7 +6834,7 @@
       <c r="D11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="16"/>
+      <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -6875,9 +6872,8 @@
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="O13" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
       <c r="T13" s="7"/>
     </row>
     <row r="14" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6893,7 +6889,7 @@
       <c r="D14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="7"/>
+      <c r="O14" s="8"/>
       <c r="P14" s="7"/>
       <c r="U14" s="7"/>
       <c r="V14" s="7"/>
@@ -7084,7 +7080,7 @@
       <c r="B26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="14" t="s">
@@ -8098,32 +8094,6 @@
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="136" priority="152">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P13">
-    <cfRule type="expression" dxfId="135" priority="137">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="138">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="139">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="132" priority="140">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="131" priority="141">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="142">
-      <formula>P$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="143">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="128" priority="144">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>